<commit_message>
added Create SKU data to resource for validation
</commit_message>
<xml_diff>
--- a/resources/SKU.xlsx
+++ b/resources/SKU.xlsx
@@ -4,54 +4,102 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15630" windowHeight="3975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>user1@uat.com</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>UAT</t>
-  </si>
-  <si>
-    <t>Yes</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+  <si>
+    <t>HSN Key</t>
+  </si>
+  <si>
+    <t>SKU Name</t>
+  </si>
+  <si>
+    <t>test SKU</t>
+  </si>
+  <si>
+    <t>SKU Local Name</t>
+  </si>
+  <si>
+    <t>test SKU Local</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is test SKU</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Biscuits And Choclates</t>
+  </si>
+  <si>
+    <t>sub-Category</t>
+  </si>
+  <si>
+    <t>Biscuits</t>
+  </si>
+  <si>
+    <t>GST Rate</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>CESS Rate</t>
+  </si>
+  <si>
+    <t>Amount Type</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>Parle Agro</t>
+  </si>
+  <si>
+    <t>variation Name</t>
+  </si>
+  <si>
+    <t>test SKU automation</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,19 +122,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,48 +428,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.42578125"/>
+    <col min="2" max="2" customWidth="true" width="19.85546875"/>
+    <col min="3" max="3" customWidth="true" width="15.0"/>
+    <col min="4" max="4" customWidth="true" width="15.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>1245.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>123456</v>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added POM structuring to SKU
</commit_message>
<xml_diff>
--- a/resources/SKU.xlsx
+++ b/resources/SKU.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5B07F6-D866-439A-85E8-39321524EB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08589161-89A1-41C6-B0ED-D6F2271BC3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,69 +19,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
-    <t>HSN Key</t>
-  </si>
-  <si>
-    <t>SKU Name</t>
-  </si>
-  <si>
     <t>test SKU</t>
   </si>
   <si>
-    <t>SKU Local Name</t>
-  </si>
-  <si>
     <t>test SKU Local</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>This is test SKU</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>sub-Category</t>
-  </si>
-  <si>
-    <t>GST Rate</t>
-  </si>
-  <si>
     <t>05</t>
   </si>
   <si>
-    <t>CESS Rate</t>
-  </si>
-  <si>
-    <t>Amount Type</t>
-  </si>
-  <si>
     <t>Net</t>
   </si>
   <si>
-    <t>Brand Name</t>
-  </si>
-  <si>
     <t>Parle Agro</t>
   </si>
   <si>
-    <t>variation Name</t>
-  </si>
-  <si>
     <t>test SKU automation</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -91,10 +52,49 @@
     <t>Beverages</t>
   </si>
   <si>
-    <t>No of Variations</t>
-  </si>
-  <si>
     <t>test SKU automation 2</t>
+  </si>
+  <si>
+    <t>itemHSNCode</t>
+  </si>
+  <si>
+    <t>skuName</t>
+  </si>
+  <si>
+    <t>localName</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subCategory</t>
+  </si>
+  <si>
+    <t>gstRate</t>
+  </si>
+  <si>
+    <t>cessAmount</t>
+  </si>
+  <si>
+    <t>amountType</t>
+  </si>
+  <si>
+    <t>brandName</t>
+  </si>
+  <si>
+    <t>numberOfVariations</t>
+  </si>
+  <si>
+    <t>variationName</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>valueText</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1">
         <v>1245</v>
@@ -497,79 +497,79 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -577,39 +577,39 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
         <v>180</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>

</xml_diff>